<commit_message>
commit after jenkin project created
</commit_message>
<xml_diff>
--- a/src/inseadTesting/TestData.xlsx
+++ b/src/inseadTesting/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="4425" windowWidth="17265" windowHeight="2445" activeTab="1"/>
+    <workbookView xWindow="3225" yWindow="4425" windowWidth="17265" windowHeight="2445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4683,7 +4683,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4694,13 +4694,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J201"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="130.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="81" style="2" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="38.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" bestFit="1" customWidth="1"/>
@@ -4962,7 +4962,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>58</v>
+        <v>452</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6896,8 +6896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DM106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9317,7 +9317,7 @@
         <v>439</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>452</v>
+        <v>58</v>
       </c>
       <c r="C24" s="41" t="s">
         <v>422</v>

</xml_diff>